<commit_message>
C25 - Update TODO_TEMPLATE.xlsx
</commit_message>
<xml_diff>
--- a/TODO_TEMPLATE.xlsx
+++ b/TODO_TEMPLATE.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="13">
   <si>
     <t>Đảm Bảo Chất Lượng Công Việc</t>
   </si>
@@ -42,6 +42,9 @@
     <t>Báo cáo hoàn thành công việc cho leader ngay sau từng task nhỏ (theo số lượng task theo leader)</t>
   </si>
   <si>
+    <t>Luôn theo dõi nội dung chat + QA dù không phải là QA của mình</t>
+  </si>
+  <si>
     <t>TODO LIST</t>
   </si>
   <si>
@@ -62,10 +65,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -128,7 +131,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -141,24 +144,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -172,9 +183,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -227,17 +237,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -248,17 +260,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -298,13 +301,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -316,7 +325,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -328,7 +343,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -340,13 +355,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -358,37 +391,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -400,7 +415,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -418,19 +439,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -442,43 +463,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -611,9 +614,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -629,6 +634,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -681,35 +701,18 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -727,130 +730,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="10" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1306,7 +1309,7 @@
   <dimension ref="B1:AB24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.62962962962963" defaultRowHeight="13.8"/>
@@ -1643,33 +1646,39 @@
       <c r="AB10" s="27"/>
     </row>
     <row r="11" ht="15" spans="2:28">
-      <c r="B11" s="10"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="12"/>
-      <c r="Q11" s="12"/>
-      <c r="R11" s="12"/>
-      <c r="S11" s="12"/>
-      <c r="T11" s="12"/>
-      <c r="U11" s="12"/>
-      <c r="V11" s="12"/>
-      <c r="W11" s="12"/>
-      <c r="X11" s="12"/>
-      <c r="Y11" s="12"/>
-      <c r="Z11" s="12"/>
-      <c r="AA11" s="12"/>
-      <c r="AB11" s="25"/>
+      <c r="B11" s="13">
+        <v>1</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="16"/>
+      <c r="S11" s="16"/>
+      <c r="T11" s="16"/>
+      <c r="U11" s="16"/>
+      <c r="V11" s="16"/>
+      <c r="W11" s="16"/>
+      <c r="X11" s="16"/>
+      <c r="Y11" s="16"/>
+      <c r="Z11" s="16"/>
+      <c r="AA11" s="26"/>
+      <c r="AB11" s="27"/>
     </row>
     <row r="12" ht="15" spans="2:28">
       <c r="B12" s="10"/>
@@ -2054,7 +2063,7 @@
     <mergeCell ref="B1:AB3"/>
   </mergeCells>
   <conditionalFormatting sqref="B6">
-    <cfRule type="dataBar" priority="16">
+    <cfRule type="dataBar" priority="18">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -2062,12 +2071,68 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{b2c7383e-cc70-44ce-a27e-5371cd2e8a0c}</x14:id>
+          <x14:id>{20a26dd0-bcc7-4109-8450-6d8ed49e5433}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
+    <cfRule type="dataBar" priority="8">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FF6DF163"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{719396f4-e605-45b5-ac5c-4b849f01394d}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB7">
+    <cfRule type="dataBar" priority="28">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FF6DF163"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{3a65ab51-e005-448f-ac26-4af95a10aa30}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8">
+    <cfRule type="dataBar" priority="7">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FF6DF163"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{5fe5d132-5093-411d-ad37-b3ef823c5738}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB8">
+    <cfRule type="dataBar" priority="27">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FF6DF163"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{f6dc5b77-4063-4d05-ad05-fcda038587d1}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9">
     <cfRule type="dataBar" priority="6">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -2076,12 +2141,12 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{5b4635f7-1191-4f1c-b19c-3920cbf5facd}</x14:id>
+          <x14:id>{c7759780-11e0-4254-92c0-1e839a27473f}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB7">
+  <conditionalFormatting sqref="AB9">
     <cfRule type="dataBar" priority="26">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -2090,12 +2155,12 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{268df280-29c3-4ef8-accc-8e7ecfa2187a}</x14:id>
+          <x14:id>{c622f5a7-773c-4bcf-8a7d-a923318d70f8}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B8">
+  <conditionalFormatting sqref="B10">
     <cfRule type="dataBar" priority="5">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -2104,12 +2169,12 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{2fcbbba3-7f52-4048-a701-4195a4c0d636}</x14:id>
+          <x14:id>{3357d704-e525-4316-a203-9ed13ef7a36d}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB8">
+  <conditionalFormatting sqref="AB10">
     <cfRule type="dataBar" priority="25">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -2118,13 +2183,13 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{240302e4-2f82-4bb7-8744-377f13f8a2fe}</x14:id>
+          <x14:id>{5d9a3724-cf48-4e88-93ec-9594ea106f29}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B9">
-    <cfRule type="dataBar" priority="4">
+  <conditionalFormatting sqref="B11">
+    <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -2132,13 +2197,13 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{94ec8158-bb09-481c-8b8d-8a0f09375be6}</x14:id>
+          <x14:id>{7fe72cb8-e394-4773-a348-08e779d9dc96}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB9">
-    <cfRule type="dataBar" priority="24">
+  <conditionalFormatting sqref="AB11">
+    <cfRule type="dataBar" priority="2">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -2146,35 +2211,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{bb8334ac-d512-4a1f-876e-781a19e0b837}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B10">
-    <cfRule type="dataBar" priority="3">
-      <dataBar>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <color rgb="FF6DF163"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{056a4c9e-8630-4ed0-9fa6-21c835dbfc45}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB10">
-    <cfRule type="dataBar" priority="23">
-      <dataBar>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <color rgb="FF6DF163"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{698ae6b7-4dce-4adb-b630-042e36284f86}</x14:id>
+          <x14:id>{e5e2ef2d-359e-4289-ab66-4e679ab2b8e3}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2186,7 +2223,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{b2c7383e-cc70-44ce-a27e-5371cd2e8a0c}">
+          <x14:cfRule type="dataBar" id="{20a26dd0-bcc7-4109-8450-6d8ed49e5433}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -2201,7 +2238,7 @@
           <xm:sqref>B6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{5b4635f7-1191-4f1c-b19c-3920cbf5facd}">
+          <x14:cfRule type="dataBar" id="{719396f4-e605-45b5-ac5c-4b849f01394d}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -2216,7 +2253,7 @@
           <xm:sqref>B7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{268df280-29c3-4ef8-accc-8e7ecfa2187a}">
+          <x14:cfRule type="dataBar" id="{3a65ab51-e005-448f-ac26-4af95a10aa30}">
             <x14:dataBar minLength="0" maxLength="100" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -2232,7 +2269,7 @@
           <xm:sqref>AB7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{2fcbbba3-7f52-4048-a701-4195a4c0d636}">
+          <x14:cfRule type="dataBar" id="{5fe5d132-5093-411d-ad37-b3ef823c5738}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -2247,7 +2284,7 @@
           <xm:sqref>B8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{240302e4-2f82-4bb7-8744-377f13f8a2fe}">
+          <x14:cfRule type="dataBar" id="{f6dc5b77-4063-4d05-ad05-fcda038587d1}">
             <x14:dataBar minLength="0" maxLength="100" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -2263,7 +2300,7 @@
           <xm:sqref>AB8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{94ec8158-bb09-481c-8b8d-8a0f09375be6}">
+          <x14:cfRule type="dataBar" id="{c7759780-11e0-4254-92c0-1e839a27473f}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -2278,7 +2315,7 @@
           <xm:sqref>B9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{bb8334ac-d512-4a1f-876e-781a19e0b837}">
+          <x14:cfRule type="dataBar" id="{c622f5a7-773c-4bcf-8a7d-a923318d70f8}">
             <x14:dataBar minLength="0" maxLength="100" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -2294,7 +2331,7 @@
           <xm:sqref>AB9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{056a4c9e-8630-4ed0-9fa6-21c835dbfc45}">
+          <x14:cfRule type="dataBar" id="{3357d704-e525-4316-a203-9ed13ef7a36d}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -2309,7 +2346,7 @@
           <xm:sqref>B10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{698ae6b7-4dce-4adb-b630-042e36284f86}">
+          <x14:cfRule type="dataBar" id="{5d9a3724-cf48-4e88-93ec-9594ea106f29}">
             <x14:dataBar minLength="0" maxLength="100" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -2323,6 +2360,37 @@
             </x14:dataBar>
           </x14:cfRule>
           <xm:sqref>AB10</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{7fe72cb8-e394-4773-a348-08e779d9dc96}">
+            <x14:dataBar minLength="0" maxLength="100">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>B11</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{e5e2ef2d-359e-4289-ab66-4e679ab2b8e3}">
+            <x14:dataBar minLength="0" maxLength="100" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>AB11</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -2352,7 +2420,7 @@
   <sheetData>
     <row r="1" spans="2:28">
       <c r="B1" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
@@ -2538,10 +2606,10 @@
       </c>
       <c r="C7" s="17"/>
       <c r="D7" s="16" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
@@ -2573,10 +2641,10 @@
       </c>
       <c r="C8" s="17"/>
       <c r="D8" s="16" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
@@ -2766,7 +2834,7 @@
     <row r="14" ht="20.1" customHeight="1" spans="2:28">
       <c r="B14" s="8"/>
       <c r="C14" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
@@ -2862,10 +2930,10 @@
       </c>
       <c r="C17" s="17"/>
       <c r="D17" s="16" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
@@ -2897,10 +2965,10 @@
       </c>
       <c r="C18" s="17"/>
       <c r="D18" s="16" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F18" s="16"/>
       <c r="G18" s="16"/>
@@ -3102,7 +3170,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{46e55592-f33f-4fe4-b122-0c63daf03b02}</x14:id>
+          <x14:id>{9122cbe8-aab8-41dd-9bf5-dcb445ce2fc4}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -3116,7 +3184,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{b018b44a-38df-42b2-ab0d-7de67cc02b24}</x14:id>
+          <x14:id>{5c8c8d0a-77c0-4e5e-9e50-ce3d1cce8fdd}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -3130,7 +3198,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{f462df61-4b7d-49e7-a283-308c37216f8e}</x14:id>
+          <x14:id>{b2788089-6ec1-4780-bf4b-fea122f6c5e6}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -3144,7 +3212,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{bb6a7324-18d7-42a7-a623-62dd3ac7c699}</x14:id>
+          <x14:id>{e0ce5518-b7d9-4e40-a0c4-3e4ba131acf3}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -3158,7 +3226,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{c32c8570-b3b8-4d9a-b7a7-d4882892b96c}</x14:id>
+          <x14:id>{452f1499-7870-4f2a-9b88-af84b7b186f3}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -3172,7 +3240,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{104e0d0f-3083-48f1-9d5d-b6a90f9606ed}</x14:id>
+          <x14:id>{1b561dcf-c051-45b6-860c-bd3c65130a94}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -3186,7 +3254,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{7074bf33-a579-43cd-bdf1-17e332630a33}</x14:id>
+          <x14:id>{2f97e042-cbe0-458e-a709-d788d5a598a5}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -3200,7 +3268,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{0ba2a5aa-0e0a-408e-8f06-5fe68140a43d}</x14:id>
+          <x14:id>{bac0a1d7-ada4-4ae9-a84b-c4333accbe18}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -3214,7 +3282,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{3f901e79-1c8c-4687-ab1a-ac10e1c33a2e}</x14:id>
+          <x14:id>{050af544-2887-4d70-a8ab-b3d2d7e5d6d4}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -3228,7 +3296,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{3cfd13c9-8a7c-42cc-95fb-0ff2c15adc08}</x14:id>
+          <x14:id>{064adacf-ef76-4564-97c1-920b3481ed6a}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -3242,7 +3310,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{3c33c294-340e-44b9-b8c4-654975045c38}</x14:id>
+          <x14:id>{d9f90afe-7247-4e3c-91d3-4b2c838a0aae}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -3256,7 +3324,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{b914e1cc-ff20-402e-be21-76cbcdc0e535}</x14:id>
+          <x14:id>{cd62dbf8-502e-4ad5-b1e0-53756ba510d7}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -3270,7 +3338,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{858d38df-a037-43bd-9b18-249b070bb68e}</x14:id>
+          <x14:id>{76564491-dc72-4b0a-a462-fb66a527e2c6}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -3284,7 +3352,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{789f85fc-133d-4a40-8f52-a060d7d7bb81}</x14:id>
+          <x14:id>{635d6a5f-83ae-4d1c-be22-7fedc93564fb}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -3298,7 +3366,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{3e3fd7e1-da55-4cb6-8ee9-9ac540678175}</x14:id>
+          <x14:id>{8064a46d-ad6f-4b25-bf2f-38e16d755c4d}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -3312,7 +3380,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{48545518-4704-4c22-8c05-0406d285e43e}</x14:id>
+          <x14:id>{2b624aa8-c326-474d-837b-77fc76f2fdac}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -3326,7 +3394,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{499286fe-2e4d-482d-9ded-94de138ae553}</x14:id>
+          <x14:id>{d5ecc3fa-0e9e-4e7b-82ec-71636fe93d5c}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -3340,7 +3408,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{105d3a79-ba3b-4eea-8d3d-cc47ee6ec418}</x14:id>
+          <x14:id>{515edd23-d681-488c-93f3-82e8085aa600}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -3354,7 +3422,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{6c4a4cd0-348f-4f25-aa96-89650b3f0822}</x14:id>
+          <x14:id>{9ba01833-b8a5-46c7-bad4-133d9efa6fcb}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -3368,7 +3436,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{9d32c295-3058-4c25-99ec-8efc018fb731}</x14:id>
+          <x14:id>{8c2a076a-1c77-4c03-af21-6d81667e9e04}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -3380,7 +3448,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{46e55592-f33f-4fe4-b122-0c63daf03b02}">
+          <x14:cfRule type="dataBar" id="{9122cbe8-aab8-41dd-9bf5-dcb445ce2fc4}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -3395,7 +3463,7 @@
           <xm:sqref>B6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{b018b44a-38df-42b2-ab0d-7de67cc02b24}">
+          <x14:cfRule type="dataBar" id="{5c8c8d0a-77c0-4e5e-9e50-ce3d1cce8fdd}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -3410,7 +3478,7 @@
           <xm:sqref>B7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{f462df61-4b7d-49e7-a283-308c37216f8e}">
+          <x14:cfRule type="dataBar" id="{b2788089-6ec1-4780-bf4b-fea122f6c5e6}">
             <x14:dataBar minLength="0" maxLength="100" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -3426,7 +3494,7 @@
           <xm:sqref>AB7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{bb6a7324-18d7-42a7-a623-62dd3ac7c699}">
+          <x14:cfRule type="dataBar" id="{e0ce5518-b7d9-4e40-a0c4-3e4ba131acf3}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -3441,7 +3509,7 @@
           <xm:sqref>B8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{c32c8570-b3b8-4d9a-b7a7-d4882892b96c}">
+          <x14:cfRule type="dataBar" id="{452f1499-7870-4f2a-9b88-af84b7b186f3}">
             <x14:dataBar minLength="0" maxLength="100" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -3457,7 +3525,7 @@
           <xm:sqref>AB8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{104e0d0f-3083-48f1-9d5d-b6a90f9606ed}">
+          <x14:cfRule type="dataBar" id="{1b561dcf-c051-45b6-860c-bd3c65130a94}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -3472,7 +3540,7 @@
           <xm:sqref>B9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{7074bf33-a579-43cd-bdf1-17e332630a33}">
+          <x14:cfRule type="dataBar" id="{2f97e042-cbe0-458e-a709-d788d5a598a5}">
             <x14:dataBar minLength="0" maxLength="100" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -3488,7 +3556,7 @@
           <xm:sqref>AB9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{0ba2a5aa-0e0a-408e-8f06-5fe68140a43d}">
+          <x14:cfRule type="dataBar" id="{bac0a1d7-ada4-4ae9-a84b-c4333accbe18}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -3503,7 +3571,7 @@
           <xm:sqref>B10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{3f901e79-1c8c-4687-ab1a-ac10e1c33a2e}">
+          <x14:cfRule type="dataBar" id="{050af544-2887-4d70-a8ab-b3d2d7e5d6d4}">
             <x14:dataBar minLength="0" maxLength="100" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -3519,7 +3587,7 @@
           <xm:sqref>AB10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{3cfd13c9-8a7c-42cc-95fb-0ff2c15adc08}">
+          <x14:cfRule type="dataBar" id="{064adacf-ef76-4564-97c1-920b3481ed6a}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -3534,7 +3602,7 @@
           <xm:sqref>B11</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{3c33c294-340e-44b9-b8c4-654975045c38}">
+          <x14:cfRule type="dataBar" id="{d9f90afe-7247-4e3c-91d3-4b2c838a0aae}">
             <x14:dataBar minLength="0" maxLength="100" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -3550,7 +3618,7 @@
           <xm:sqref>AB11</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{b914e1cc-ff20-402e-be21-76cbcdc0e535}">
+          <x14:cfRule type="dataBar" id="{cd62dbf8-502e-4ad5-b1e0-53756ba510d7}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -3565,7 +3633,7 @@
           <xm:sqref>B12</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{858d38df-a037-43bd-9b18-249b070bb68e}">
+          <x14:cfRule type="dataBar" id="{76564491-dc72-4b0a-a462-fb66a527e2c6}">
             <x14:dataBar minLength="0" maxLength="100" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -3581,7 +3649,7 @@
           <xm:sqref>AB12</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{789f85fc-133d-4a40-8f52-a060d7d7bb81}">
+          <x14:cfRule type="dataBar" id="{635d6a5f-83ae-4d1c-be22-7fedc93564fb}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -3596,7 +3664,7 @@
           <xm:sqref>B16</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{3e3fd7e1-da55-4cb6-8ee9-9ac540678175}">
+          <x14:cfRule type="dataBar" id="{8064a46d-ad6f-4b25-bf2f-38e16d755c4d}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -3611,7 +3679,7 @@
           <xm:sqref>B17</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{48545518-4704-4c22-8c05-0406d285e43e}">
+          <x14:cfRule type="dataBar" id="{2b624aa8-c326-474d-837b-77fc76f2fdac}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -3626,7 +3694,7 @@
           <xm:sqref>B18</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{499286fe-2e4d-482d-9ded-94de138ae553}">
+          <x14:cfRule type="dataBar" id="{d5ecc3fa-0e9e-4e7b-82ec-71636fe93d5c}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -3641,7 +3709,7 @@
           <xm:sqref>B19</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{105d3a79-ba3b-4eea-8d3d-cc47ee6ec418}">
+          <x14:cfRule type="dataBar" id="{515edd23-d681-488c-93f3-82e8085aa600}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -3656,7 +3724,7 @@
           <xm:sqref>B20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{6c4a4cd0-348f-4f25-aa96-89650b3f0822}">
+          <x14:cfRule type="dataBar" id="{9ba01833-b8a5-46c7-bad4-133d9efa6fcb}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -3671,7 +3739,7 @@
           <xm:sqref>B21</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{9d32c295-3058-4c25-99ec-8efc018fb731}">
+          <x14:cfRule type="dataBar" id="{8c2a076a-1c77-4c03-af21-6d81667e9e04}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>

</xml_diff>